<commit_message>
new model run with disaggregated zones
</commit_message>
<xml_diff>
--- a/input/estimation_results_splineGC_distVoT_knots2040.xlsx
+++ b/input/estimation_results_splineGC_distVoT_knots2040.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="31">
   <si>
     <t>Value</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>mu_pt</t>
+  </si>
+  <si>
+    <t>Active bound</t>
   </si>
 </sst>
 </file>
@@ -501,22 +504,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-4.797235132265175</v>
+        <v>-4.882132119955108</v>
       </c>
       <c r="C2">
-        <v>0.3812816533657314</v>
+        <v>0.2383130824720972</v>
       </c>
       <c r="D2">
-        <v>-12.58186721002175</v>
+        <v>-20.48621111905063</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.460460262845462</v>
+        <v>0.4009764595860811</v>
       </c>
       <c r="G2">
-        <v>-10.41834772586056</v>
+        <v>-12.1756078274391</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -527,22 +530,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.83013581316388</v>
+        <v>-2.305972066520545</v>
       </c>
       <c r="C3">
-        <v>0.07574225102056514</v>
+        <v>0.0394989374988297</v>
       </c>
       <c r="D3">
-        <v>-37.36535124095343</v>
+        <v>-58.38061002498783</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.09134400678583612</v>
+        <v>0.04760688188500999</v>
       </c>
       <c r="G3">
-        <v>-30.98326767950279</v>
+        <v>-48.43778830317867</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -553,22 +556,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-4.810541823222757</v>
+        <v>-5.334386493712358</v>
       </c>
       <c r="C4">
-        <v>0.1037287369361899</v>
+        <v>0.08674067448547841</v>
       </c>
       <c r="D4">
-        <v>-46.37617274933199</v>
+        <v>-61.49809792642791</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1210850609125466</v>
+        <v>0.1138062051059339</v>
       </c>
       <c r="G4">
-        <v>-39.72861546229191</v>
+        <v>-46.87254520741612</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -579,22 +582,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.267555036559449</v>
+        <v>-2.757348058088943</v>
       </c>
       <c r="C5">
-        <v>0.05498823015506313</v>
+        <v>0.0283003796845227</v>
       </c>
       <c r="D5">
-        <v>-59.42280788716354</v>
+        <v>-97.43148639086704</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.05574407862780803</v>
+        <v>0.02975962701943817</v>
       </c>
       <c r="G5">
-        <v>-58.61707856678832</v>
+        <v>-92.65398576023549</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -605,22 +608,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.422174011607091</v>
+        <v>-1.612799075475201</v>
       </c>
       <c r="C6">
-        <v>0.06701635749231324</v>
+        <v>0.03545607130472861</v>
       </c>
       <c r="D6">
-        <v>-36.14302690033421</v>
+        <v>-45.48724706733398</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.1013260045206901</v>
+        <v>0.05398446036133046</v>
       </c>
       <c r="G6">
-        <v>-23.90476189271333</v>
+        <v>-29.87524677806103</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -631,25 +634,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.5500108370000311</v>
+        <v>0.5896198298575183</v>
       </c>
       <c r="C7">
-        <v>0.08567723914746553</v>
+        <v>0.04527543415644584</v>
       </c>
       <c r="D7">
-        <v>6.419567699343884</v>
+        <v>13.02295253139112</v>
       </c>
       <c r="E7">
-        <v>1.36661792993209E-10</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.1046858687072178</v>
+        <v>0.0543953966603254</v>
       </c>
       <c r="G7">
-        <v>5.253916730043905</v>
+        <v>10.83951705581682</v>
       </c>
       <c r="H7">
-        <v>1.488982208641687E-07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -657,25 +660,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.1909058960368964</v>
+        <v>-0.5777376675969722</v>
       </c>
       <c r="C8">
-        <v>0.008883581872959985</v>
+        <v>0.008038717425928052</v>
       </c>
       <c r="D8">
-        <v>-21.48974352541056</v>
+        <v>-71.86938375685891</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.03103490276251036</v>
+        <v>0.03250306371803684</v>
       </c>
       <c r="G8">
-        <v>-6.151328956877142</v>
+        <v>-17.77486801271505</v>
       </c>
       <c r="H8">
-        <v>7.683635949717882E-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -691,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>36255</v>
+        <v>97331</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -699,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>59175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -707,7 +710,7 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>-70420.87323906925</v>
+        <v>-189046.3796197089</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -718,7 +721,7 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>-15536.67605408924</v>
+        <v>-48767.4617277893</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -729,7 +732,7 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>109768.39436996</v>
+        <v>280557.8357838392</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -740,7 +743,7 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.7793739932570227</v>
+        <v>0.7420344053882898</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -751,7 +754,7 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.7792745909111268</v>
+        <v>0.7419973774377198</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -762,7 +765,7 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>31087.35210817849</v>
+        <v>97548.9234555786</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -773,7 +776,7 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>31146.84043625112</v>
+        <v>97615.32456531643</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -784,7 +787,7 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.1048554101047105</v>
+        <v>164.2977122766904</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
@@ -839,22 +842,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-5.195710354751928</v>
+        <v>-5.805484519088056</v>
       </c>
       <c r="C2">
-        <v>0.3624655003095752</v>
+        <v>0.2810919808140378</v>
       </c>
       <c r="D2">
-        <v>-14.33435830531283</v>
+        <v>-20.65332672342863</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.3597826370831717</v>
+        <v>0.5415205755068808</v>
       </c>
       <c r="G2">
-        <v>-14.44124818494458</v>
+        <v>-10.72070902135886</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -865,22 +868,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.767684349297109</v>
+        <v>-2.206019047772801</v>
       </c>
       <c r="C3">
-        <v>0.06102712941043411</v>
+        <v>0.03640723017818813</v>
       </c>
       <c r="D3">
-        <v>-45.35170466045064</v>
+        <v>-60.59288325356993</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.06868545407835798</v>
+        <v>0.04143104184960195</v>
       </c>
       <c r="G3">
-        <v>-40.29505790468633</v>
+        <v>-53.24556055772939</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -891,22 +894,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-3.517144309334741</v>
+        <v>-5.02751331139807</v>
       </c>
       <c r="C4">
-        <v>0.08431350571914625</v>
+        <v>0.0795229644307736</v>
       </c>
       <c r="D4">
-        <v>-41.71507612375385</v>
+        <v>-63.22089911241457</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1063421273545615</v>
+        <v>0.1285147838677973</v>
       </c>
       <c r="G4">
-        <v>-33.0738569636474</v>
+        <v>-39.12011645733968</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -917,22 +920,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.273511089790335</v>
+        <v>-2.675561890289109</v>
       </c>
       <c r="C5">
-        <v>0.0546512743494816</v>
+        <v>0.02703123913405355</v>
       </c>
       <c r="D5">
-        <v>-59.89816575652066</v>
+        <v>-98.98036405288119</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.05527008764253779</v>
+        <v>0.03047363954359879</v>
       </c>
       <c r="G5">
-        <v>-59.22753571447074</v>
+        <v>-87.79922353748293</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -943,22 +946,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.87254190962033</v>
+        <v>-2.437658924719382</v>
       </c>
       <c r="C6">
-        <v>0.05754164984702698</v>
+        <v>0.03354954322776975</v>
       </c>
       <c r="D6">
-        <v>-49.92109050152212</v>
+        <v>-72.65848325176822</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.06151702065133511</v>
+        <v>0.03711321037436997</v>
       </c>
       <c r="G6">
-        <v>-46.69507526870105</v>
+        <v>-65.68170471188357</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -969,25 +972,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.6714054162116251</v>
+        <v>0.5227205486189287</v>
       </c>
       <c r="C7">
-        <v>0.0719320565699144</v>
+        <v>0.04186307279758915</v>
       </c>
       <c r="D7">
-        <v>9.333883225750013</v>
+        <v>12.48643526829286</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.08188348397573161</v>
+        <v>0.04864315629169372</v>
       </c>
       <c r="G7">
-        <v>8.19952185242404</v>
+        <v>10.74602448665915</v>
       </c>
       <c r="H7">
-        <v>2.220446049250313E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -995,25 +998,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.05701578002998374</v>
+        <v>-0.4478997346693834</v>
       </c>
       <c r="C8">
-        <v>0.004702236523458058</v>
+        <v>0.008272220380466681</v>
       </c>
       <c r="D8">
-        <v>-12.12524715538</v>
+        <v>-54.14504378135474</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.008985301763150318</v>
+        <v>0.03365876322829559</v>
       </c>
       <c r="G8">
-        <v>-6.345449661335977</v>
+        <v>-13.30707642557858</v>
       </c>
       <c r="H8">
-        <v>2.217765970868868E-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1021,22 +1024,22 @@
         <v>29</v>
       </c>
       <c r="B9">
-        <v>3.429120846099743</v>
+        <v>1.305216225942577</v>
       </c>
       <c r="C9">
-        <v>0.2529883407742534</v>
+        <v>0.02606299490031045</v>
       </c>
       <c r="D9">
-        <v>13.55446197878193</v>
+        <v>50.07928793045308</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.346998873401039</v>
+        <v>0.06114447648377627</v>
       </c>
       <c r="G9">
-        <v>9.882224724506774</v>
+        <v>21.34642899901018</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1055,7 +1058,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>36255</v>
+        <v>97331</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1063,7 +1066,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>59175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1071,7 +1074,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-70420.87323906925</v>
+        <v>-189046.3796197089</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -1082,7 +1085,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-11995.81072847164</v>
+        <v>-38632.55532067006</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -1093,7 +1096,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>116850.1250211952</v>
+        <v>300827.6485980777</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -1104,7 +1107,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.8296554675238477</v>
+        <v>0.7956450930275184</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1115,7 +1118,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8295418648428239</v>
+        <v>0.7956027753697241</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1126,7 +1129,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>24007.62145694327</v>
+        <v>77281.11064134011</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1137,7 +1140,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>24075.60811759772</v>
+        <v>77356.99762389765</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1148,7 +1151,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.1857052311163814</v>
+        <v>1.020828729332048</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1169,244 +1172,271 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-11.84792757096133</v>
+        <v>-17.10654667617357</v>
       </c>
       <c r="C2">
-        <v>1.442951196879259</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>-8.210899714824331</v>
+        <v>1.539232131225374</v>
       </c>
       <c r="E2">
-        <v>2.220446049250313E-16</v>
+        <v>-11.11368865627509</v>
       </c>
       <c r="F2">
-        <v>2.608576610314056</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>-4.541912828672844</v>
+        <v>3.208648253667866</v>
       </c>
       <c r="H2">
-        <v>5.57460928907183E-06</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>-5.331387339394015</v>
+      </c>
+      <c r="I2">
+        <v>9.746527962484208E-08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.517457216786155</v>
+        <v>-2.66251528662669</v>
       </c>
       <c r="C3">
-        <v>0.07696129453028627</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>-32.71069220120082</v>
+        <v>0.0818862590149779</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-32.51479941390028</v>
       </c>
       <c r="F3">
-        <v>0.09148066972884512</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>-27.51900728588966</v>
+        <v>0.1000332274108088</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>-26.61630895594798</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-5.855222977692572</v>
+        <v>-6.648090726498597</v>
       </c>
       <c r="C4">
-        <v>0.2008723010737059</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>-29.14898144938421</v>
+        <v>0.2522235298294457</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-26.35793231104986</v>
       </c>
       <c r="F4">
-        <v>0.2947269541447803</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>-19.86660159632457</v>
+        <v>0.4431301093497786</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-15.00257054582364</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-4.755272146199376</v>
+        <v>-3.801423129409171</v>
       </c>
       <c r="C5">
-        <v>0.118164161001321</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>-40.24293073215503</v>
+        <v>0.0877970282256945</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-43.29785650189757</v>
       </c>
       <c r="F5">
-        <v>0.1703197180708335</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>-27.91968070438988</v>
+        <v>0.08909295223006046</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-42.66805661117771</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.318657631332258</v>
+        <v>-2.237963868279847</v>
       </c>
       <c r="C6">
-        <v>0.06828389059148858</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>-33.95614413952671</v>
+        <v>0.07104777050493268</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-31.49942429403145</v>
       </c>
       <c r="F6">
-        <v>0.08337365548341832</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>-27.81043505755127</v>
+        <v>0.08998387298793126</v>
       </c>
       <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>-24.87072176344316</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.9403122574412532</v>
+        <v>0.9084413589640341</v>
       </c>
       <c r="C7">
-        <v>0.08445244718855048</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>11.13422155005041</v>
+        <v>0.08629808682190761</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>10.52678445628551</v>
       </c>
       <c r="F7">
-        <v>0.0996390792823504</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>9.437183324192116</v>
+        <v>0.100989889339605</v>
       </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>8.995369387020141</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.5342673199902079</v>
+        <v>-0.8255134837763529</v>
       </c>
       <c r="C8">
-        <v>0.0216696770732238</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>-24.65506607158336</v>
+        <v>0.03181625262509406</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-25.94628265948754</v>
       </c>
       <c r="F8">
-        <v>0.05165035057137991</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>-10.34392436992</v>
+        <v>0.09811128199814731</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>-8.414052563210229</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B9">
-        <v>1.369842486633793</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.06060368049862983</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>22.60328870067162</v>
+        <v>0.04178266294406235</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>23.93337163164484</v>
       </c>
       <c r="F9">
-        <v>0.1005323197925471</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>13.62589154871312</v>
+        <v>0.09253482947713847</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>10.80674169553702</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1414,61 +1444,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>24760</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>24829</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>70670</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>72502</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-48083.15791028061</v>
+        <v>-48214.80514900837</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-10064.26672144368</v>
+        <v>-10177.87405490344</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>76037.78237767387</v>
+        <v>76073.86218820987</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.7906903964123403</v>
+        <v>0.7889056271523112</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1479,7 +1509,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.7905240179890485</v>
+        <v>0.7887397030139625</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1490,7 +1520,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>20144.53344288736</v>
+        <v>20371.74810980688</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1501,7 +1531,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>20209.46932070175</v>
+        <v>20436.70625063752</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1512,7 +1542,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.08971509186729475</v>
+        <v>33.76725336386561</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1533,244 +1563,271 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-8.46448644447916</v>
+        <v>-12.62456409053915</v>
       </c>
       <c r="C2">
-        <v>9.395423887166579</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>-0.9009158656525325</v>
+        <v>9.387336914250024</v>
       </c>
       <c r="E2">
-        <v>0.3676330548998252</v>
+        <v>-1.3448504305172</v>
       </c>
       <c r="F2">
-        <v>0.6359351902749675</v>
+        <v>0.1786735406656241</v>
       </c>
       <c r="G2">
-        <v>-13.31029729746401</v>
+        <v>0.8636616710502926</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>-14.61748797441308</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.785486718510311</v>
+        <v>0.8113270670153896</v>
       </c>
       <c r="C3">
-        <v>0.09194252245888726</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>8.543236551526492</v>
+        <v>0.09936573375419061</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>8.165058882596668</v>
       </c>
       <c r="F3">
-        <v>0.08703933815558622</v>
+        <v>2.220446049250313E-16</v>
       </c>
       <c r="G3">
-        <v>9.024502427927736</v>
+        <v>0.09605889672311371</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>8.446141843102888</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-1.825439261252443</v>
+        <v>-2.521383544285894</v>
       </c>
       <c r="C4">
-        <v>0.1973649680395264</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>-9.249054071677309</v>
+        <v>0.2227015416606506</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-11.32180552269342</v>
       </c>
       <c r="F4">
-        <v>0.2164159779163035</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>-8.43486363081016</v>
+        <v>0.2392466674080101</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-10.5388449987725</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.323499462915839</v>
+        <v>-2.049170855308743</v>
       </c>
       <c r="C5">
-        <v>0.1768639947503213</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>-18.79127217276541</v>
+        <v>0.1132520902826716</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-18.09388992462845</v>
       </c>
       <c r="F5">
-        <v>0.2127766822093988</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>-15.6196601451145</v>
+        <v>0.09592190651896632</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-21.36290790783612</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.07694039441578068</v>
+        <v>0.09517416739426034</v>
       </c>
       <c r="C6">
-        <v>0.09446450507263815</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0.8144899966036728</v>
+        <v>0.1037716106357957</v>
       </c>
       <c r="E6">
-        <v>0.4153643005989085</v>
+        <v>0.9171503343847133</v>
       </c>
       <c r="F6">
-        <v>0.1036052813240647</v>
+        <v>0.3590638681491547</v>
       </c>
       <c r="G6">
-        <v>0.7426300419485419</v>
+        <v>0.1273666286293825</v>
       </c>
       <c r="H6">
-        <v>0.4577056950230773</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.7472457143480077</v>
+      </c>
+      <c r="I6">
+        <v>0.4549152541924537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.2729847441520188</v>
+        <v>0.2667881734507485</v>
       </c>
       <c r="C7">
-        <v>0.1112533181494237</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>2.453722268178774</v>
+        <v>0.1208210303095646</v>
       </c>
       <c r="E7">
-        <v>0.0141386132485577</v>
+        <v>2.208126952461757</v>
       </c>
       <c r="F7">
-        <v>0.1045553953452269</v>
+        <v>0.02723542465360551</v>
       </c>
       <c r="G7">
-        <v>2.610910161552757</v>
+        <v>0.1164661799991907</v>
       </c>
       <c r="H7">
-        <v>0.009030161246072588</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>2.290692228873672</v>
+      </c>
+      <c r="I7">
+        <v>0.02198122040284556</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.5471407442706029</v>
+        <v>-1.236944868624151</v>
       </c>
       <c r="C8">
-        <v>0.03342932706395863</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>-16.36708819246605</v>
+        <v>0.06021607222790262</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-20.54177270052798</v>
       </c>
       <c r="F8">
-        <v>0.04641173765053511</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>-11.78884420123181</v>
+        <v>0.1003883356819519</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>-12.3215995187231</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B9">
-        <v>1.514528053868792</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.1017013094128881</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>14.8919228534226</v>
+        <v>0.05417461492442847</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>18.45882986699512</v>
       </c>
       <c r="F9">
-        <v>0.1214800599790372</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>12.46729754768101</v>
+        <v>0.07038869115374902</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>14.20682759700296</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1778,61 +1835,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>3985</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>4265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>91445</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>93066</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-7735.799711726274</v>
+        <v>-8279.113046663488</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-3225.497044970734</v>
+        <v>-3263.216514312843</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>9020.605333511079</v>
+        <v>10031.79306470129</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.5830428442864957</v>
+        <v>0.6058495039359402</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1843,7 +1900,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.5820086913484519</v>
+        <v>0.6048832168524194</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1854,7 +1911,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>6466.994089941469</v>
+        <v>6542.433028625686</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1865,7 +1922,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>6517.316430671263</v>
+        <v>6593.298608305093</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1876,7 +1933,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.0165050681749558</v>
+        <v>26.85179298487392</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1931,25 +1988,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-8.030116588556394</v>
+        <v>-14.03041334263573</v>
       </c>
       <c r="C2">
-        <v>1.197816556747523</v>
+        <v>1.242178545899047</v>
       </c>
       <c r="D2">
-        <v>-6.703961924153795</v>
+        <v>-11.29500536694666</v>
       </c>
       <c r="E2">
-        <v>2.028421874911146E-11</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1.566965118276524</v>
+        <v>1.767097317819981</v>
       </c>
       <c r="G2">
-        <v>-5.124630085823845</v>
+        <v>-7.93980795576367</v>
       </c>
       <c r="H2">
-        <v>2.981224620501877E-07</v>
+        <v>1.998401444325282E-15</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1957,22 +2014,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.971604404420002</v>
+        <v>-2.831530983253771</v>
       </c>
       <c r="C3">
-        <v>0.09633758139243927</v>
+        <v>0.1016602223634194</v>
       </c>
       <c r="D3">
-        <v>-30.84574432396139</v>
+        <v>-27.85288992514191</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.1136884755874876</v>
+        <v>0.1205916109047962</v>
       </c>
       <c r="G3">
-        <v>-26.13813219910087</v>
+        <v>-23.48033135977583</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1983,25 +2040,25 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-6.075893027409444</v>
+        <v>-8.716929721533047</v>
       </c>
       <c r="C4">
-        <v>0.277474332905955</v>
+        <v>0.4907174019660649</v>
       </c>
       <c r="D4">
-        <v>-21.89713536303468</v>
+        <v>-17.76364499528357</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.3806801874913813</v>
+        <v>1.126365813259211</v>
       </c>
       <c r="G4">
-        <v>-15.96062318727056</v>
+        <v>-7.73898641002789</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>9.992007221626409E-15</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2009,22 +2066,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-4.120611269084836</v>
+        <v>-2.909861411913836</v>
       </c>
       <c r="C5">
-        <v>0.08768194144777743</v>
+        <v>0.0597271895750063</v>
       </c>
       <c r="D5">
-        <v>-46.99498210288871</v>
+        <v>-48.71920866558753</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.09192947850924033</v>
+        <v>0.05513327983911157</v>
       </c>
       <c r="G5">
-        <v>-44.82361192411911</v>
+        <v>-52.7786741584269</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2035,22 +2092,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-3.132737472696292</v>
+        <v>-3.012977654126399</v>
       </c>
       <c r="C6">
-        <v>0.08904266973193792</v>
+        <v>0.09404171092751873</v>
       </c>
       <c r="D6">
-        <v>-35.18242975112233</v>
+        <v>-32.03873711366872</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.1029544493685999</v>
+        <v>0.1141624663885616</v>
       </c>
       <c r="G6">
-        <v>-30.4283835415446</v>
+        <v>-26.39201612788807</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2061,25 +2118,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.8445803499966196</v>
+        <v>0.7204470755283175</v>
       </c>
       <c r="C7">
-        <v>0.1117415058210979</v>
+        <v>0.1166170033616506</v>
       </c>
       <c r="D7">
-        <v>7.558340509110578</v>
+        <v>6.177890485610231</v>
       </c>
       <c r="E7">
-        <v>4.085620730620576E-14</v>
+        <v>6.496374549413986E-10</v>
       </c>
       <c r="F7">
-        <v>0.1330446510807412</v>
+        <v>0.1407689889746293</v>
       </c>
       <c r="G7">
-        <v>6.348096997030466</v>
+        <v>5.117938835649115</v>
       </c>
       <c r="H7">
-        <v>2.179947333758037E-10</v>
+        <v>3.088927338357195E-07</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2087,22 +2144,22 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.3730152499226352</v>
+        <v>-0.896565591070378</v>
       </c>
       <c r="C8">
-        <v>0.02064129656803797</v>
+        <v>0.02787722864299906</v>
       </c>
       <c r="D8">
-        <v>-18.07130907174847</v>
+        <v>-32.16121668878792</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.03212278495292786</v>
+        <v>0.06018358067303147</v>
       </c>
       <c r="G8">
-        <v>-11.6121703167781</v>
+        <v>-14.89717928119443</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -2113,22 +2170,22 @@
         <v>29</v>
       </c>
       <c r="B9">
-        <v>2.488335162675109</v>
+        <v>1.496761165243692</v>
       </c>
       <c r="C9">
-        <v>0.1891842960476835</v>
+        <v>0.08873063616589609</v>
       </c>
       <c r="D9">
-        <v>13.1529689020696</v>
+        <v>16.86859499626779</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.2518123816172062</v>
+        <v>0.1580395967993169</v>
       </c>
       <c r="G9">
-        <v>9.881702983365463</v>
+        <v>9.470798429992971</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -2147,7 +2204,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>25300</v>
+        <v>26154</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2155,7 +2212,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>70130</v>
+        <v>71177</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2163,7 +2220,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-49165.08782809578</v>
+        <v>-50809.01361652932</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -2174,7 +2231,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-5929.626367506788</v>
+        <v>-6219.252810948139</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -2185,7 +2242,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>86470.92292117797</v>
+        <v>89179.52161116234</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -2196,7 +2253,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.8793935569028262</v>
+        <v>0.8775954822133198</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -2207,7 +2264,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8792308398132529</v>
+        <v>0.8774380298356693</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -2218,7 +2275,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>11875.25273501358</v>
+        <v>12454.50562189628</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -2229,7 +2286,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>11940.3612124113</v>
+        <v>12519.87968126801</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -2240,7 +2297,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.06663521964168904</v>
+        <v>0.08804379537337213</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -2295,22 +2352,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-3.058792142635145</v>
+        <v>-2.974920240276819</v>
       </c>
       <c r="C2">
-        <v>0.2746535836429931</v>
+        <v>0.2753874869519544</v>
       </c>
       <c r="D2">
-        <v>-11.13690963745479</v>
+        <v>-10.80267035079862</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.2921834872212611</v>
+        <v>0.2881968806532013</v>
       </c>
       <c r="G2">
-        <v>-10.46873720251966</v>
+        <v>-10.32252754968802</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2321,22 +2378,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.911927254614276</v>
+        <v>-2.796028354539394</v>
       </c>
       <c r="C3">
-        <v>0.1494854244412892</v>
+        <v>0.1488419804693228</v>
       </c>
       <c r="D3">
-        <v>-19.4796734564442</v>
+        <v>-18.78521332303605</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.1597252282975632</v>
+        <v>0.1671698611250261</v>
       </c>
       <c r="G3">
-        <v>-18.23085360810657</v>
+        <v>-16.72567253285117</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2347,22 +2404,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-3.375953127065558</v>
+        <v>-3.525824553571377</v>
       </c>
       <c r="C4">
-        <v>0.1874561622709018</v>
+        <v>0.2101283867817738</v>
       </c>
       <c r="D4">
-        <v>-18.00929393927743</v>
+        <v>-16.77938239364621</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1686565374283186</v>
+        <v>0.267980218164326</v>
       </c>
       <c r="G4">
-        <v>-20.01673447434782</v>
+        <v>-13.15703292475617</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -2373,22 +2430,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.912513498584697</v>
+        <v>-3.007300833621382</v>
       </c>
       <c r="C5">
-        <v>0.2231124860991382</v>
+        <v>0.1568224358818245</v>
       </c>
       <c r="D5">
-        <v>-17.53605800818428</v>
+        <v>-19.1764706160257</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.2264566144444027</v>
+        <v>0.1539244786163734</v>
       </c>
       <c r="G5">
-        <v>-17.27709966954954</v>
+        <v>-19.53750865784312</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2399,22 +2456,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.890303006776957</v>
+        <v>-2.806720058985937</v>
       </c>
       <c r="C6">
-        <v>0.1370715472098121</v>
+        <v>0.1352456957502868</v>
       </c>
       <c r="D6">
-        <v>-21.0860901887453</v>
+        <v>-20.7527496044545</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.1394704800431272</v>
+        <v>0.1422371847093756</v>
       </c>
       <c r="G6">
-        <v>-20.72340330285818</v>
+        <v>-19.73267443897131</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2425,25 +2482,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.8436903350877569</v>
+        <v>0.727864362921456</v>
       </c>
       <c r="C7">
-        <v>0.171947669320287</v>
+        <v>0.1730114259508508</v>
       </c>
       <c r="D7">
-        <v>4.906669211760089</v>
+        <v>4.207030598824312</v>
       </c>
       <c r="E7">
-        <v>9.263607110288063E-07</v>
+        <v>2.58748117900609E-05</v>
       </c>
       <c r="F7">
-        <v>0.1866315702361862</v>
+        <v>0.1966424244418309</v>
       </c>
       <c r="G7">
-        <v>4.52061960374683</v>
+        <v>3.701461497881229</v>
       </c>
       <c r="H7">
-        <v>6.16588968727072E-06</v>
+        <v>0.0002143611875069507</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2451,25 +2508,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.03408319493629643</v>
+        <v>-0.05151379277912382</v>
       </c>
       <c r="C8">
-        <v>0.004759880888217959</v>
+        <v>0.009027856024848652</v>
       </c>
       <c r="D8">
-        <v>-7.160514251661612</v>
+        <v>-5.706093743335637</v>
       </c>
       <c r="E8">
-        <v>8.038014698286133E-13</v>
+        <v>1.15598348671142E-08</v>
       </c>
       <c r="F8">
-        <v>0.005453468851901994</v>
+        <v>0.01983959659601226</v>
       </c>
       <c r="G8">
-        <v>-6.249819309852539</v>
+        <v>-2.596514124157042</v>
       </c>
       <c r="H8">
-        <v>4.109277362829289E-10</v>
+        <v>0.009417503375376723</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2477,25 +2534,25 @@
         <v>29</v>
       </c>
       <c r="B9">
-        <v>5.99247696978721</v>
+        <v>4.22953893943911</v>
       </c>
       <c r="C9">
-        <v>1.314515228794576</v>
+        <v>0.8332103199829526</v>
       </c>
       <c r="D9">
-        <v>4.558697258518924</v>
+        <v>5.076196055187658</v>
       </c>
       <c r="E9">
-        <v>5.147190559995352E-06</v>
+        <v>3.850659759940811E-07</v>
       </c>
       <c r="F9">
-        <v>1.0029411433838</v>
+        <v>1.158965207044106</v>
       </c>
       <c r="G9">
-        <v>5.974903920652141</v>
+        <v>3.649409761166496</v>
       </c>
       <c r="H9">
-        <v>2.302258383934941E-09</v>
+        <v>0.0002628435508784666</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2511,7 +2568,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>5130</v>
+        <v>5191</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2519,7 +2576,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>90300</v>
+        <v>92140</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2527,7 +2584,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-9970.495311627261</v>
+        <v>-10088.4250773205</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -2538,7 +2595,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-1771.049922694262</v>
+        <v>-1905.202011357622</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -2549,7 +2606,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>16398.890777866</v>
+        <v>16366.44613192576</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -2560,7 +2617,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.8223709186614909</v>
+        <v>0.8111497090224071</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -2571,7 +2628,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8215685513015994</v>
+        <v>0.8103567210249065</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -2582,7 +2639,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>3558.099845388525</v>
+        <v>3826.404022715243</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -2593,7 +2650,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>3610.442732893844</v>
+        <v>3878.841475801861</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -2604,7 +2661,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.03297307332348595</v>
+        <v>0.01409117255908978</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -2659,22 +2716,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-5.195710354751928</v>
+        <v>-5.489505650950972</v>
       </c>
       <c r="C2">
-        <v>0.3624655003095752</v>
+        <v>0.4106501632218189</v>
       </c>
       <c r="D2">
-        <v>-14.33435830531283</v>
+        <v>-13.36783993431833</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.3597826370831717</v>
+        <v>0.6043311728221061</v>
       </c>
       <c r="G2">
-        <v>-14.44124818494458</v>
+        <v>-9.083604979892192</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2685,22 +2742,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.767684349297109</v>
+        <v>-2.802437390378705</v>
       </c>
       <c r="C3">
-        <v>0.06102712941043411</v>
+        <v>0.07084290842038503</v>
       </c>
       <c r="D3">
-        <v>-45.35170466045064</v>
+        <v>-39.5584745582284</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.06868545407835798</v>
+        <v>0.08119792734995487</v>
       </c>
       <c r="G3">
-        <v>-40.29505790468633</v>
+        <v>-34.5136567131878</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2711,22 +2768,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-3.517144309334741</v>
+        <v>-4.681377200405231</v>
       </c>
       <c r="C4">
-        <v>0.08431350571914625</v>
+        <v>0.106174051007834</v>
       </c>
       <c r="D4">
-        <v>-41.71507612375385</v>
+        <v>-44.0915379602481</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1063421273545615</v>
+        <v>0.1650457894461455</v>
       </c>
       <c r="G4">
-        <v>-33.0738569636474</v>
+        <v>-28.36411165722446</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -2737,22 +2794,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.273511089790335</v>
+        <v>-2.301393048779851</v>
       </c>
       <c r="C5">
-        <v>0.0546512743494816</v>
+        <v>0.03819745036079281</v>
       </c>
       <c r="D5">
-        <v>-59.89816575652066</v>
+        <v>-60.24991267851953</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.05527008764253779</v>
+        <v>0.04229958414336105</v>
       </c>
       <c r="G5">
-        <v>-59.22753571447074</v>
+        <v>-54.4069899358823</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2763,22 +2820,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.87254190962033</v>
+        <v>-2.950787895162701</v>
       </c>
       <c r="C6">
-        <v>0.05754164984702698</v>
+        <v>0.06355719680645171</v>
       </c>
       <c r="D6">
-        <v>-49.92109050152212</v>
+        <v>-46.42728193549225</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.06151702065133511</v>
+        <v>0.06937968206856263</v>
       </c>
       <c r="G6">
-        <v>-46.69507526870105</v>
+        <v>-42.53100918287091</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2789,25 +2846,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.6714054162116251</v>
+        <v>0.6322131924877474</v>
       </c>
       <c r="C7">
-        <v>0.0719320565699144</v>
+        <v>0.08084259404532729</v>
       </c>
       <c r="D7">
-        <v>9.333883225750013</v>
+        <v>7.820298197423929</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>5.329070518200751E-15</v>
       </c>
       <c r="F7">
-        <v>0.08188348397573161</v>
+        <v>0.09638449312714355</v>
       </c>
       <c r="G7">
-        <v>8.19952185242404</v>
+        <v>6.559283262026153</v>
       </c>
       <c r="H7">
-        <v>2.220446049250313E-16</v>
+        <v>5.406697312082542E-11</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2815,25 +2872,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.05701578002998374</v>
+        <v>-0.2395905233409181</v>
       </c>
       <c r="C8">
-        <v>0.004702236523458058</v>
+        <v>0.00915706628875748</v>
       </c>
       <c r="D8">
-        <v>-12.12524715538</v>
+        <v>-26.16455049965878</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.008985301763150318</v>
+        <v>0.03398467083682616</v>
       </c>
       <c r="G8">
-        <v>-6.345449661335977</v>
+        <v>-7.049958626678686</v>
       </c>
       <c r="H8">
-        <v>2.217765970868868E-10</v>
+        <v>1.789679515695752E-12</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2841,22 +2898,22 @@
         <v>29</v>
       </c>
       <c r="B9">
-        <v>3.429120846099743</v>
+        <v>1.399265923475132</v>
       </c>
       <c r="C9">
-        <v>0.2529883407742534</v>
+        <v>0.05293987828825491</v>
       </c>
       <c r="D9">
-        <v>13.55446197878193</v>
+        <v>26.43122668050351</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.346998873401039</v>
+        <v>0.1150446431353724</v>
       </c>
       <c r="G9">
-        <v>9.882224724506774</v>
+        <v>12.16280815290655</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -2875,7 +2932,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>36255</v>
+        <v>36892</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2883,7 +2940,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>59175</v>
+        <v>60439</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2891,7 +2948,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-70420.87323906925</v>
+        <v>-71655.02273022372</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -2902,7 +2959,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-11995.81072847164</v>
+        <v>-13095.14459895685</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -2913,7 +2970,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>116850.1250211952</v>
+        <v>117119.7562625337</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -2924,7 +2981,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.8296554675238477</v>
+        <v>0.8172473596406608</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -2935,7 +2992,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8295418648428239</v>
+        <v>0.8171357135941566</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -2946,7 +3003,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>24007.62145694327</v>
+        <v>26206.28919791371</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -2957,7 +3014,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>24075.60811759772</v>
+        <v>26274.41519794855</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -2968,7 +3025,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.1857052311163814</v>
+        <v>0.2312089853213282</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
introduced node clustering for short-distance modes
</commit_message>
<xml_diff>
--- a/input/estimation_results_splineGC_distVoT_knots2040.xlsx
+++ b/input/estimation_results_splineGC_distVoT_knots2040.xlsx
@@ -504,22 +504,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-4.882132119955108</v>
+        <v>-4.383404289443892</v>
       </c>
       <c r="C2">
-        <v>0.2383130824720972</v>
+        <v>0.2596183643857707</v>
       </c>
       <c r="D2">
-        <v>-20.48621111905063</v>
+        <v>-16.88403014099006</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.4009764595860811</v>
+        <v>0.3894117726006704</v>
       </c>
       <c r="G2">
-        <v>-12.1756078274391</v>
+        <v>-11.25647604377625</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -530,22 +530,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.305972066520545</v>
+        <v>-3.187337517652953</v>
       </c>
       <c r="C3">
-        <v>0.0394989374988297</v>
+        <v>0.04066067010727931</v>
       </c>
       <c r="D3">
-        <v>-58.38061002498783</v>
+        <v>-78.38871098886139</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.04760688188500999</v>
+        <v>0.05023641008557603</v>
       </c>
       <c r="G3">
-        <v>-48.43778830317867</v>
+        <v>-63.44676126784201</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -556,22 +556,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-5.334386493712358</v>
+        <v>-4.820397241866983</v>
       </c>
       <c r="C4">
-        <v>0.08674067448547841</v>
+        <v>0.07619906729277523</v>
       </c>
       <c r="D4">
-        <v>-61.49809792642791</v>
+        <v>-63.26058064918107</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1138062051059339</v>
+        <v>0.08160730427501645</v>
       </c>
       <c r="G4">
-        <v>-46.87254520741612</v>
+        <v>-59.06820822830092</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -582,22 +582,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.757348058088943</v>
+        <v>-2.277599482901801</v>
       </c>
       <c r="C5">
-        <v>0.0283003796845227</v>
+        <v>0.02746498144280618</v>
       </c>
       <c r="D5">
-        <v>-97.43148639086704</v>
+        <v>-82.92739930098756</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.02975962701943817</v>
+        <v>0.02692210013079303</v>
       </c>
       <c r="G5">
-        <v>-92.65398576023549</v>
+        <v>-84.59962156877658</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -608,22 +608,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-1.612799075475201</v>
+        <v>-1.894592494488386</v>
       </c>
       <c r="C6">
-        <v>0.03545607130472861</v>
+        <v>0.03469442531680163</v>
       </c>
       <c r="D6">
-        <v>-45.48724706733398</v>
+        <v>-54.60798030774363</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.05398446036133046</v>
+        <v>0.04402497736582386</v>
       </c>
       <c r="G6">
-        <v>-29.87524677806103</v>
+        <v>-43.03449105141706</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -634,22 +634,22 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.5896198298575183</v>
+        <v>0.5598116427237861</v>
       </c>
       <c r="C7">
-        <v>0.04527543415644584</v>
+        <v>0.04596044022349604</v>
       </c>
       <c r="D7">
-        <v>13.02295253139112</v>
+        <v>12.18029331315233</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.0543953966603254</v>
+        <v>0.05564499801734789</v>
       </c>
       <c r="G7">
-        <v>10.83951705581682</v>
+        <v>10.06041266367301</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -660,22 +660,22 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.5777376675969722</v>
+        <v>-0.4079928433400677</v>
       </c>
       <c r="C8">
-        <v>0.008038717425928052</v>
+        <v>0.006165987072778744</v>
       </c>
       <c r="D8">
-        <v>-71.86938375685891</v>
+        <v>-66.16829366075899</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.03250306371803684</v>
+        <v>0.01845629992557268</v>
       </c>
       <c r="G8">
-        <v>-17.77486801271505</v>
+        <v>-22.10588498156995</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -694,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>97331</v>
+        <v>83104</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -710,7 +710,7 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>-189046.3796197089</v>
+        <v>-161393.2085171241</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -721,7 +721,7 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>-48767.4617277893</v>
+        <v>-45722.09496909202</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -732,7 +732,7 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>280557.8357838392</v>
+        <v>231342.2270960641</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -743,7 +743,7 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.7420344053882898</v>
+        <v>0.7167037238482012</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -754,7 +754,7 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.7419973774377198</v>
+        <v>0.7166603515151005</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -765,7 +765,7 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>97548.9234555786</v>
+        <v>91458.18993818405</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -776,7 +776,7 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>97615.32456531643</v>
+        <v>91523.48487498528</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -787,7 +787,7 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>164.2977122766904</v>
+        <v>0.2753763476878969</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
@@ -842,22 +842,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-5.805484519088056</v>
+        <v>-4.485960889141351</v>
       </c>
       <c r="C2">
-        <v>0.2810919808140378</v>
+        <v>0.2640529609395687</v>
       </c>
       <c r="D2">
-        <v>-20.65332672342863</v>
+        <v>-16.98886796489289</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.5415205755068808</v>
+        <v>0.4362831163170282</v>
       </c>
       <c r="G2">
-        <v>-10.72070902135886</v>
+        <v>-10.28222436616501</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -868,22 +868,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.206019047772801</v>
+        <v>-3.234006223435477</v>
       </c>
       <c r="C3">
-        <v>0.03640723017818813</v>
+        <v>0.04215135864246253</v>
       </c>
       <c r="D3">
-        <v>-60.59288325356993</v>
+        <v>-76.72365322472895</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.04143104184960195</v>
+        <v>0.06301767801507945</v>
       </c>
       <c r="G3">
-        <v>-53.24556055772939</v>
+        <v>-51.31903182249295</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -894,22 +894,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-5.02751331139807</v>
+        <v>-4.78042782230465</v>
       </c>
       <c r="C4">
-        <v>0.0795229644307736</v>
+        <v>0.08988668847676802</v>
       </c>
       <c r="D4">
-        <v>-63.22089911241457</v>
+        <v>-53.18282276624522</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1285147838677973</v>
+        <v>0.1382896512362178</v>
       </c>
       <c r="G4">
-        <v>-39.12011645733968</v>
+        <v>-34.56822531238451</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -920,22 +920,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.675561890289109</v>
+        <v>-2.270208873747357</v>
       </c>
       <c r="C5">
-        <v>0.02703123913405355</v>
+        <v>0.02749166022745055</v>
       </c>
       <c r="D5">
-        <v>-98.98036405288119</v>
+        <v>-82.57809295491522</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.03047363954359879</v>
+        <v>0.03123874921571106</v>
       </c>
       <c r="G5">
-        <v>-87.79922353748293</v>
+        <v>-72.67284800908705</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -946,22 +946,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.437658924719382</v>
+        <v>-2.689053849866395</v>
       </c>
       <c r="C6">
-        <v>0.03354954322776975</v>
+        <v>0.03556355563957669</v>
       </c>
       <c r="D6">
-        <v>-72.65848325176822</v>
+        <v>-75.61262650784832</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.03711321037436997</v>
+        <v>0.04034629622552877</v>
       </c>
       <c r="G6">
-        <v>-65.68170471188357</v>
+        <v>-66.64933591016762</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -972,22 +972,22 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.5227205486189287</v>
+        <v>0.6132434008265686</v>
       </c>
       <c r="C7">
-        <v>0.04186307279758915</v>
+        <v>0.04420347623705406</v>
       </c>
       <c r="D7">
-        <v>12.48643526829286</v>
+        <v>13.87319398903995</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.04864315629169372</v>
+        <v>0.05300871333035609</v>
       </c>
       <c r="G7">
-        <v>10.74602448665915</v>
+        <v>11.5687282768923</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -998,22 +998,22 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.4478997346693834</v>
+        <v>-0.3694125081132953</v>
       </c>
       <c r="C8">
-        <v>0.008272220380466681</v>
+        <v>0.007635600497331688</v>
       </c>
       <c r="D8">
-        <v>-54.14504378135474</v>
+        <v>-48.38028236841215</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.03365876322829559</v>
+        <v>0.02702556186991355</v>
       </c>
       <c r="G8">
-        <v>-13.30707642557858</v>
+        <v>-13.66900380800397</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1024,22 +1024,22 @@
         <v>29</v>
       </c>
       <c r="B9">
-        <v>1.305216225942577</v>
+        <v>1.061228085796776</v>
       </c>
       <c r="C9">
-        <v>0.02606299490031045</v>
+        <v>0.02122852572012728</v>
       </c>
       <c r="D9">
-        <v>50.07928793045308</v>
+        <v>49.99066349626911</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.06114447648377627</v>
+        <v>0.04993485721228887</v>
       </c>
       <c r="G9">
-        <v>21.34642899901018</v>
+        <v>21.2522503325715</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1058,7 +1058,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>97331</v>
+        <v>83104</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1074,7 +1074,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-189046.3796197089</v>
+        <v>-161393.2085171241</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -1085,7 +1085,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-38632.55532067006</v>
+        <v>-36504.47781558963</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -1096,7 +1096,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>300827.6485980777</v>
+        <v>249777.4614030689</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -1107,7 +1107,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.7956450930275184</v>
+        <v>0.7738165183591573</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1118,7 +1118,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.7956027753697241</v>
+        <v>0.7737669499784707</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1129,7 +1129,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>77281.11064134011</v>
+        <v>73024.95563117927</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1140,7 +1140,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>77356.99762389765</v>
+        <v>73099.57841609497</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1151,7 +1151,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.020828729332048</v>
+        <v>0.3782377315898401</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1209,28 +1209,28 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-17.10654667617357</v>
+        <v>-12.54774788236644</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.539232131225374</v>
+        <v>1.60770296139357</v>
       </c>
       <c r="E2">
-        <v>-11.11368865627509</v>
+        <v>-7.804767537089032</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>5.995204332975845E-15</v>
       </c>
       <c r="G2">
-        <v>3.208648253667866</v>
+        <v>3.535111192972774</v>
       </c>
       <c r="H2">
-        <v>-5.331387339394015</v>
+        <v>-3.549463424887262</v>
       </c>
       <c r="I2">
-        <v>9.746527962484208E-08</v>
+        <v>0.000386017085419299</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1238,25 +1238,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.66251528662669</v>
+        <v>-3.628172181241371</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.0818862590149779</v>
+        <v>0.09556933814220658</v>
       </c>
       <c r="E3">
-        <v>-32.51479941390028</v>
+        <v>-37.9637680010159</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.1000332274108088</v>
+        <v>0.1657601451831271</v>
       </c>
       <c r="H3">
-        <v>-26.61630895594798</v>
+        <v>-21.88808520427554</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1267,25 +1267,25 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-6.648090726498597</v>
+        <v>-5.787127120453888</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.2522235298294457</v>
+        <v>0.2585127006887729</v>
       </c>
       <c r="E4">
-        <v>-26.35793231104986</v>
+        <v>-22.38623907078783</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.4431301093497786</v>
+        <v>0.4662168690177352</v>
       </c>
       <c r="H4">
-        <v>-15.00257054582364</v>
+        <v>-12.41295093557359</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1296,25 +1296,25 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.801423129409171</v>
+        <v>-3.407534080809495</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.0877970282256945</v>
+        <v>0.08514754958491191</v>
       </c>
       <c r="E5">
-        <v>-43.29785650189757</v>
+        <v>-40.01916787295671</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.08909295223006046</v>
+        <v>0.09632132528120828</v>
       </c>
       <c r="H5">
-        <v>-42.66805661117771</v>
+        <v>-35.37673584599531</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1325,25 +1325,25 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.237963868279847</v>
+        <v>-2.45372564302903</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.07104777050493268</v>
+        <v>0.06969733565757841</v>
       </c>
       <c r="E6">
-        <v>-31.49942429403145</v>
+        <v>-35.20544393668267</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.08998387298793126</v>
+        <v>0.08084425942694701</v>
       </c>
       <c r="H6">
-        <v>-24.87072176344316</v>
+        <v>-30.35126625467181</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1354,25 +1354,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.9084413589640341</v>
+        <v>0.9986389472538022</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.08629808682190761</v>
+        <v>0.08734629872039557</v>
       </c>
       <c r="E7">
-        <v>10.52678445628551</v>
+        <v>11.43309976362648</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.100989889339605</v>
+        <v>0.1071953629061339</v>
       </c>
       <c r="H7">
-        <v>8.995369387020141</v>
+        <v>9.316064801499525</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1383,28 +1383,28 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.8255134837763529</v>
+        <v>-0.5605407835529395</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.03181625262509406</v>
+        <v>0.03481501129416414</v>
       </c>
       <c r="E8">
-        <v>-25.94628265948754</v>
+        <v>-16.10054866323998</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.09811128199814731</v>
+        <v>0.1051970398251126</v>
       </c>
       <c r="H8">
-        <v>-8.414052563210229</v>
+        <v>-5.328484380214731</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>9.903571251967946E-08</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1418,22 +1418,22 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.04178266294406235</v>
+        <v>0.05332912186784602</v>
       </c>
       <c r="E9">
-        <v>23.93337163164484</v>
+        <v>18.75148071025964</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.09253482947713847</v>
+        <v>0.136535925184964</v>
       </c>
       <c r="H9">
-        <v>10.80674169553702</v>
+        <v>7.324079714883164</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>2.404743071338089E-13</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1449,7 +1449,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>24829</v>
+        <v>22194</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1457,7 +1457,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>72502</v>
+        <v>60910</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1465,7 +1465,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-48214.80514900837</v>
+        <v>-43096.42679635662</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -1476,7 +1476,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-10177.87405490344</v>
+        <v>-9759.279273798624</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -1487,7 +1487,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>76073.86218820987</v>
+        <v>66674.29504511598</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -1498,7 +1498,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.7889056271523112</v>
+        <v>0.7735478321691469</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1509,7 +1509,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.7887397030139625</v>
+        <v>0.773362201930292</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1520,7 +1520,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>20371.74810980688</v>
+        <v>19534.55854759725</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1531,7 +1531,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>20436.70625063752</v>
+        <v>19598.61916568573</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1542,7 +1542,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>33.76725336386561</v>
+        <v>185.1374633162337</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1562,6 +1562,370 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>-9.034814335534838</v>
+      </c>
+      <c r="C2">
+        <v>46.86582028925071</v>
+      </c>
+      <c r="D2">
+        <v>-0.1927804587601999</v>
+      </c>
+      <c r="E2">
+        <v>0.8471309080618032</v>
+      </c>
+      <c r="F2">
+        <v>0.5533200460079453</v>
+      </c>
+      <c r="G2">
+        <v>-16.32836981186311</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>-0.1267575033074903</v>
+      </c>
+      <c r="C3">
+        <v>0.08997557041731816</v>
+      </c>
+      <c r="D3">
+        <v>-1.408799107575232</v>
+      </c>
+      <c r="E3">
+        <v>0.1588945791244762</v>
+      </c>
+      <c r="F3">
+        <v>0.0894278747867441</v>
+      </c>
+      <c r="G3">
+        <v>-1.417427212821114</v>
+      </c>
+      <c r="H3">
+        <v>0.156358061149833</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>-1.855779418335967</v>
+      </c>
+      <c r="C4">
+        <v>0.2293184610554567</v>
+      </c>
+      <c r="D4">
+        <v>-8.092586221774702</v>
+      </c>
+      <c r="E4">
+        <v>6.661338147750939E-16</v>
+      </c>
+      <c r="F4">
+        <v>0.2554057608317103</v>
+      </c>
+      <c r="G4">
+        <v>-7.266004542312422</v>
+      </c>
+      <c r="H4">
+        <v>3.703704010149522E-13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>-1.464163499296202</v>
+      </c>
+      <c r="C5">
+        <v>0.1005303836353698</v>
+      </c>
+      <c r="D5">
+        <v>-14.56438786314412</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.08524908386185058</v>
+      </c>
+      <c r="G5">
+        <v>-17.17512298042915</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>-0.1301133094087085</v>
+      </c>
+      <c r="C6">
+        <v>0.08989388426620049</v>
+      </c>
+      <c r="D6">
+        <v>-1.44741002650867</v>
+      </c>
+      <c r="E6">
+        <v>0.147782119228596</v>
+      </c>
+      <c r="F6">
+        <v>0.09079805663589034</v>
+      </c>
+      <c r="G6">
+        <v>-1.432996632631428</v>
+      </c>
+      <c r="H6">
+        <v>0.1518587996491145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0.4502095296808979</v>
+      </c>
+      <c r="C7">
+        <v>0.1132366795664817</v>
+      </c>
+      <c r="D7">
+        <v>3.975827721233897</v>
+      </c>
+      <c r="E7">
+        <v>7.01348862246487E-05</v>
+      </c>
+      <c r="F7">
+        <v>0.1138604869881988</v>
+      </c>
+      <c r="G7">
+        <v>3.95404535488734</v>
+      </c>
+      <c r="H7">
+        <v>7.684083365999683E-05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>-0.7128431681645684</v>
+      </c>
+      <c r="C8">
+        <v>0.04247139023961548</v>
+      </c>
+      <c r="D8">
+        <v>-16.78407897982249</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.06505822312642234</v>
+      </c>
+      <c r="G8">
+        <v>-10.95700334113581</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>1.310938164639942</v>
+      </c>
+      <c r="C9">
+        <v>0.08706833266654851</v>
+      </c>
+      <c r="D9">
+        <v>15.05642895058678</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.1070091840058691</v>
+      </c>
+      <c r="G9">
+        <v>12.25070704742539</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>3583</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>79521</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>-6955.5477906438</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>-3312.840596084012</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>7285.414389119576</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>0.5237124816336891</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>0.5225623206052852</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>6641.681192168024</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>6691.152837906463</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>0.02807544568379191</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I21"/>
   <sheetViews>
@@ -1600,28 +1964,28 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-12.62456409053915</v>
+        <v>-7.697798076187872</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>9.387336914250024</v>
+        <v>1.157894783613168</v>
       </c>
       <c r="E2">
-        <v>-1.3448504305172</v>
+        <v>-6.648098069987997</v>
       </c>
       <c r="F2">
-        <v>0.1786735406656241</v>
+        <v>2.969047230294564E-11</v>
       </c>
       <c r="G2">
-        <v>0.8636616710502926</v>
+        <v>1.163417238494138</v>
       </c>
       <c r="H2">
-        <v>-14.61748797441308</v>
+        <v>-6.616541187022011</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>3.677014248637533E-11</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1629,25 +1993,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.8113270670153896</v>
+        <v>-3.90560534574583</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.09936573375419061</v>
+        <v>0.1146952593987984</v>
       </c>
       <c r="E3">
-        <v>8.165058882596668</v>
+        <v>-34.05202068697483</v>
       </c>
       <c r="F3">
-        <v>2.220446049250313E-16</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.09605889672311371</v>
+        <v>0.1391223123358284</v>
       </c>
       <c r="H3">
-        <v>8.446141843102888</v>
+        <v>-28.07317733706193</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1658,25 +2022,25 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-2.521383544285894</v>
+        <v>-6.435328939012436</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.2227015416606506</v>
+        <v>0.3492565219030974</v>
       </c>
       <c r="E4">
-        <v>-11.32180552269342</v>
+        <v>-18.42579461063849</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.2392466674080101</v>
+        <v>0.398079977563546</v>
       </c>
       <c r="H4">
-        <v>-10.5388449987725</v>
+        <v>-16.16591966870566</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1687,25 +2051,25 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.049170855308743</v>
+        <v>-2.456761855015613</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.1132520902826716</v>
+        <v>0.06045729554705288</v>
       </c>
       <c r="E5">
-        <v>-18.09388992462845</v>
+        <v>-40.63631746649264</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.09592190651896632</v>
+        <v>0.05362876264304614</v>
       </c>
       <c r="H5">
-        <v>-21.36290790783612</v>
+        <v>-45.81052655210147</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1716,28 +2080,28 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.09517416739426034</v>
+        <v>-3.461169820587383</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.1037716106357957</v>
+        <v>0.1003707981527896</v>
       </c>
       <c r="E6">
-        <v>0.9171503343847133</v>
+        <v>-34.4838327908742</v>
       </c>
       <c r="F6">
-        <v>0.3590638681491547</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.1273666286293825</v>
+        <v>0.1139509132523858</v>
       </c>
       <c r="H6">
-        <v>0.7472457143480077</v>
+        <v>-30.37421747486449</v>
       </c>
       <c r="I6">
-        <v>0.4549152541924537</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1745,28 +2109,28 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.2667881734507485</v>
+        <v>0.8692088486740241</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.1208210303095646</v>
+        <v>0.1232640125487827</v>
       </c>
       <c r="E7">
-        <v>2.208126952461757</v>
+        <v>7.051602740337762</v>
       </c>
       <c r="F7">
-        <v>0.02723542465360551</v>
+        <v>1.768585278227874E-12</v>
       </c>
       <c r="G7">
-        <v>0.1164661799991907</v>
+        <v>0.1530653539661918</v>
       </c>
       <c r="H7">
-        <v>2.290692228873672</v>
+        <v>5.678677938222452</v>
       </c>
       <c r="I7">
-        <v>0.02198122040284556</v>
+        <v>1.357397794166104E-08</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1774,25 +2138,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-1.236944868624151</v>
+        <v>-0.745304966739618</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.06021607222790262</v>
+        <v>0.02543438490505471</v>
       </c>
       <c r="E8">
-        <v>-20.54177270052798</v>
+        <v>-29.30304662455193</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.1003883356819519</v>
+        <v>0.0375277391597263</v>
       </c>
       <c r="H8">
-        <v>-12.3215995187231</v>
+        <v>-19.86010837390007</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1809,19 +2173,19 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.05417461492442847</v>
+        <v>0.0452437566571564</v>
       </c>
       <c r="E9">
-        <v>18.45882986699512</v>
+        <v>22.10249709319453</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.07038869115374902</v>
+        <v>0.0594876833106687</v>
       </c>
       <c r="H9">
-        <v>14.20682759700296</v>
+        <v>16.81020245447442</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1840,7 +2204,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>4265</v>
+        <v>20767</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1848,7 +2212,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>93066</v>
+        <v>62337</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1856,7 +2220,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-8279.113046663488</v>
+        <v>-40333.4865748387</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -1867,7 +2231,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-3263.216514312843</v>
+        <v>-5801.590710266214</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -1878,7 +2242,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>10031.79306470129</v>
+        <v>69063.79172914497</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -1889,7 +2253,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.6058495039359402</v>
+        <v>0.8561594545142688</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1900,7 +2264,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.6048832168524194</v>
+        <v>0.8559611081604233</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1911,7 +2275,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>6542.433028625686</v>
+        <v>11619.18142053243</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1922,7 +2286,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>6593.298608305093</v>
+        <v>11682.71038427117</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1933,371 +2297,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>26.85179298487392</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>-14.03041334263573</v>
-      </c>
-      <c r="C2">
-        <v>1.242178545899047</v>
-      </c>
-      <c r="D2">
-        <v>-11.29500536694666</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1.767097317819981</v>
-      </c>
-      <c r="G2">
-        <v>-7.93980795576367</v>
-      </c>
-      <c r="H2">
-        <v>1.998401444325282E-15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>-2.831530983253771</v>
-      </c>
-      <c r="C3">
-        <v>0.1016602223634194</v>
-      </c>
-      <c r="D3">
-        <v>-27.85288992514191</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0.1205916109047962</v>
-      </c>
-      <c r="G3">
-        <v>-23.48033135977583</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>-8.716929721533047</v>
-      </c>
-      <c r="C4">
-        <v>0.4907174019660649</v>
-      </c>
-      <c r="D4">
-        <v>-17.76364499528357</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1.126365813259211</v>
-      </c>
-      <c r="G4">
-        <v>-7.73898641002789</v>
-      </c>
-      <c r="H4">
-        <v>9.992007221626409E-15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>-2.909861411913836</v>
-      </c>
-      <c r="C5">
-        <v>0.0597271895750063</v>
-      </c>
-      <c r="D5">
-        <v>-48.71920866558753</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0.05513327983911157</v>
-      </c>
-      <c r="G5">
-        <v>-52.7786741584269</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>-3.012977654126399</v>
-      </c>
-      <c r="C6">
-        <v>0.09404171092751873</v>
-      </c>
-      <c r="D6">
-        <v>-32.03873711366872</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0.1141624663885616</v>
-      </c>
-      <c r="G6">
-        <v>-26.39201612788807</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>0.7204470755283175</v>
-      </c>
-      <c r="C7">
-        <v>0.1166170033616506</v>
-      </c>
-      <c r="D7">
-        <v>6.177890485610231</v>
-      </c>
-      <c r="E7">
-        <v>6.496374549413986E-10</v>
-      </c>
-      <c r="F7">
-        <v>0.1407689889746293</v>
-      </c>
-      <c r="G7">
-        <v>5.117938835649115</v>
-      </c>
-      <c r="H7">
-        <v>3.088927338357195E-07</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>-0.896565591070378</v>
-      </c>
-      <c r="C8">
-        <v>0.02787722864299906</v>
-      </c>
-      <c r="D8">
-        <v>-32.16121668878792</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0.06018358067303147</v>
-      </c>
-      <c r="G8">
-        <v>-14.89717928119443</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9">
-        <v>1.496761165243692</v>
-      </c>
-      <c r="C9">
-        <v>0.08873063616589609</v>
-      </c>
-      <c r="D9">
-        <v>16.86859499626779</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0.1580395967993169</v>
-      </c>
-      <c r="G9">
-        <v>9.470798429992971</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>26154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>71177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <v>-50809.01361652932</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>-6219.252810948139</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <v>89179.52161116234</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16">
-        <v>0.8775954822133198</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <v>0.8774380298356693</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>12454.50562189628</v>
-      </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <v>12519.87968126801</v>
-      </c>
-      <c r="C19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20">
-        <v>0.08804379537337213</v>
+        <v>42.18340496796686</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -2352,25 +2352,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-2.974920240276819</v>
+        <v>-2.361195328069249</v>
       </c>
       <c r="C2">
-        <v>0.2753874869519544</v>
+        <v>0.2850460091031438</v>
       </c>
       <c r="D2">
-        <v>-10.80267035079862</v>
+        <v>-8.283558627950658</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2.220446049250313E-16</v>
       </c>
       <c r="F2">
-        <v>0.2881968806532013</v>
+        <v>0.316639349701074</v>
       </c>
       <c r="G2">
-        <v>-10.32252754968802</v>
+        <v>-7.457049574850235</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>8.837375276016246E-14</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2378,22 +2378,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.796028354539394</v>
+        <v>-3.338720760317815</v>
       </c>
       <c r="C3">
-        <v>0.1488419804693228</v>
+        <v>0.1767744470314344</v>
       </c>
       <c r="D3">
-        <v>-18.78521332303605</v>
+        <v>-18.88689692647782</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.1671698611250261</v>
+        <v>0.1979339962782788</v>
       </c>
       <c r="G3">
-        <v>-16.72567253285117</v>
+        <v>-16.86784899560079</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2404,22 +2404,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-3.525824553571377</v>
+        <v>-3.526929234928152</v>
       </c>
       <c r="C4">
-        <v>0.2101283867817738</v>
+        <v>0.2196436249121606</v>
       </c>
       <c r="D4">
-        <v>-16.77938239364621</v>
+        <v>-16.05750786683945</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.267980218164326</v>
+        <v>0.2394011520593723</v>
       </c>
       <c r="G4">
-        <v>-13.15703292475617</v>
+        <v>-14.73229850645606</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -2430,22 +2430,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.007300833621382</v>
+        <v>-2.701688198111595</v>
       </c>
       <c r="C5">
-        <v>0.1568224358818245</v>
+        <v>0.1596319346096212</v>
       </c>
       <c r="D5">
-        <v>-19.1764706160257</v>
+        <v>-16.92448446934227</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.1539244786163734</v>
+        <v>0.1630635450222024</v>
       </c>
       <c r="G5">
-        <v>-19.53750865784312</v>
+        <v>-16.56831511754352</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2456,22 +2456,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.806720058985937</v>
+        <v>-2.872933837663979</v>
       </c>
       <c r="C6">
-        <v>0.1352456957502868</v>
+        <v>0.1368130480752328</v>
       </c>
       <c r="D6">
-        <v>-20.7527496044545</v>
+        <v>-20.99897544921423</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.1422371847093756</v>
+        <v>0.1491125584552034</v>
       </c>
       <c r="G6">
-        <v>-19.73267443897131</v>
+        <v>-19.26688045210538</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2482,25 +2482,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.727864362921456</v>
+        <v>0.8567632351232968</v>
       </c>
       <c r="C7">
-        <v>0.1730114259508508</v>
+        <v>0.1726259576335742</v>
       </c>
       <c r="D7">
-        <v>4.207030598824312</v>
+        <v>4.963119375951046</v>
       </c>
       <c r="E7">
-        <v>2.58748117900609E-05</v>
+        <v>6.936991490125166E-07</v>
       </c>
       <c r="F7">
-        <v>0.1966424244418309</v>
+        <v>0.2051216200544875</v>
       </c>
       <c r="G7">
-        <v>3.701461497881229</v>
+        <v>4.176854857599655</v>
       </c>
       <c r="H7">
-        <v>0.0002143611875069507</v>
+        <v>2.955674888149851E-05</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2508,25 +2508,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.05151379277912382</v>
+        <v>-0.04301540467211686</v>
       </c>
       <c r="C8">
-        <v>0.009027856024848652</v>
+        <v>0.006306444949947622</v>
       </c>
       <c r="D8">
-        <v>-5.706093743335637</v>
+        <v>-6.820864213279801</v>
       </c>
       <c r="E8">
-        <v>1.15598348671142E-08</v>
+        <v>9.049427873719651E-12</v>
       </c>
       <c r="F8">
-        <v>0.01983959659601226</v>
+        <v>0.009783235513790962</v>
       </c>
       <c r="G8">
-        <v>-2.596514124157042</v>
+        <v>-4.396848528432142</v>
       </c>
       <c r="H8">
-        <v>0.009417503375376723</v>
+        <v>1.098339356730982E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2534,25 +2534,25 @@
         <v>29</v>
       </c>
       <c r="B9">
-        <v>4.22953893943911</v>
+        <v>3.284547650362089</v>
       </c>
       <c r="C9">
-        <v>0.8332103199829526</v>
+        <v>0.5799014561452674</v>
       </c>
       <c r="D9">
-        <v>5.076196055187658</v>
+        <v>5.663975517832288</v>
       </c>
       <c r="E9">
-        <v>3.850659759940811E-07</v>
+        <v>1.47905518943503E-08</v>
       </c>
       <c r="F9">
-        <v>1.158965207044106</v>
+        <v>0.6570122514064681</v>
       </c>
       <c r="G9">
-        <v>3.649409761166496</v>
+        <v>4.999218269264915</v>
       </c>
       <c r="H9">
-        <v>0.0002628435508784666</v>
+        <v>5.756321208583159E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2568,7 +2568,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>5191</v>
+        <v>4806</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2576,7 +2576,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>92140</v>
+        <v>78298</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2584,7 +2584,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-10088.4250773205</v>
+        <v>-9340.174574013135</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -2595,7 +2595,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-1905.202011357622</v>
+        <v>-1894.331019713707</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -2606,7 +2606,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>16366.44613192576</v>
+        <v>14891.68710859886</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -2617,7 +2617,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.8111497090224071</v>
+        <v>0.7971846238308818</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -2628,7 +2628,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8103567210249065</v>
+        <v>0.7963281087907607</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -2639,7 +2639,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>3826.404022715243</v>
+        <v>3804.662039427414</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -2650,7 +2650,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>3878.841475801861</v>
+        <v>3856.483002757785</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -2661,7 +2661,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.01409117255908978</v>
+        <v>0.02807051344189841</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -2716,25 +2716,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-5.489505650950972</v>
+        <v>-4.846085610566901</v>
       </c>
       <c r="C2">
-        <v>0.4106501632218189</v>
+        <v>0.4387699154848498</v>
       </c>
       <c r="D2">
-        <v>-13.36783993431833</v>
+        <v>-11.0447080338493</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.6043311728221061</v>
+        <v>0.7104140701955383</v>
       </c>
       <c r="G2">
-        <v>-9.083604979892192</v>
+        <v>-6.821494412734586</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>9.009903934042995E-12</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2742,22 +2742,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.802437390378705</v>
+        <v>-3.712375798763819</v>
       </c>
       <c r="C3">
-        <v>0.07084290842038503</v>
+        <v>0.08209070786614932</v>
       </c>
       <c r="D3">
-        <v>-39.5584745582284</v>
+        <v>-45.22285037201687</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.08119792734995487</v>
+        <v>0.1352098480056674</v>
       </c>
       <c r="G3">
-        <v>-34.5136567131878</v>
+        <v>-27.45640094653618</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2768,22 +2768,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-4.681377200405231</v>
+        <v>-4.427085406598698</v>
       </c>
       <c r="C4">
-        <v>0.106174051007834</v>
+        <v>0.1232827990322417</v>
       </c>
       <c r="D4">
-        <v>-44.0915379602481</v>
+        <v>-35.91000075720943</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1650457894461455</v>
+        <v>0.2154381851062926</v>
       </c>
       <c r="G4">
-        <v>-28.36411165722446</v>
+        <v>-20.54921417210449</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -2794,22 +2794,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.301393048779851</v>
+        <v>-1.877398325242114</v>
       </c>
       <c r="C5">
-        <v>0.03819745036079281</v>
+        <v>0.04012773910606553</v>
       </c>
       <c r="D5">
-        <v>-60.24991267851953</v>
+        <v>-46.78554952422763</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.04229958414336105</v>
+        <v>0.0493043212592728</v>
       </c>
       <c r="G5">
-        <v>-54.4069899358823</v>
+        <v>-38.07776432758472</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2820,22 +2820,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.950787895162701</v>
+        <v>-3.063132233202988</v>
       </c>
       <c r="C6">
-        <v>0.06355719680645171</v>
+        <v>0.0667914218948069</v>
       </c>
       <c r="D6">
-        <v>-46.42728193549225</v>
+        <v>-45.861162201746</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.06937968206856263</v>
+        <v>0.07804961537402753</v>
       </c>
       <c r="G6">
-        <v>-42.53100918287091</v>
+        <v>-39.24596192465418</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2846,25 +2846,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.6322131924877474</v>
+        <v>0.634637226729197</v>
       </c>
       <c r="C7">
-        <v>0.08084259404532729</v>
+        <v>0.08431998914834715</v>
       </c>
       <c r="D7">
-        <v>7.820298197423929</v>
+        <v>7.526533543696942</v>
       </c>
       <c r="E7">
-        <v>5.329070518200751E-15</v>
+        <v>5.218048215738236E-14</v>
       </c>
       <c r="F7">
-        <v>0.09638449312714355</v>
+        <v>0.1025466486602843</v>
       </c>
       <c r="G7">
-        <v>6.559283262026153</v>
+        <v>6.188766137366597</v>
       </c>
       <c r="H7">
-        <v>5.406697312082542E-11</v>
+        <v>6.06369621181102E-10</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2872,25 +2872,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.2395905233409181</v>
+        <v>-0.2329989742715633</v>
       </c>
       <c r="C8">
-        <v>0.00915706628875748</v>
+        <v>0.01032995625044918</v>
       </c>
       <c r="D8">
-        <v>-26.16455049965878</v>
+        <v>-22.55565934864746</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.03398467083682616</v>
+        <v>0.04037872723267039</v>
       </c>
       <c r="G8">
-        <v>-7.049958626678686</v>
+        <v>-5.770339736787047</v>
       </c>
       <c r="H8">
-        <v>1.789679515695752E-12</v>
+        <v>7.911187260845054E-09</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2898,22 +2898,22 @@
         <v>29</v>
       </c>
       <c r="B9">
-        <v>1.399265923475132</v>
+        <v>1.144762455691204</v>
       </c>
       <c r="C9">
-        <v>0.05293987828825491</v>
+        <v>0.04614421733481777</v>
       </c>
       <c r="D9">
-        <v>26.43122668050351</v>
+        <v>24.80836216995348</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.1150446431353724</v>
+        <v>0.1251271869380919</v>
       </c>
       <c r="G9">
-        <v>12.16280815290655</v>
+        <v>9.148790792024984</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -2932,7 +2932,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>36892</v>
+        <v>31754</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2940,7 +2940,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>60439</v>
+        <v>51350</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2948,7 +2948,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-71655.02273022372</v>
+        <v>-61667.57278128399</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -2959,7 +2959,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-13095.14459895685</v>
+        <v>-12373.04832477327</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -2970,7 +2970,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>117119.7562625337</v>
+        <v>98589.04891302144</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -2981,7 +2981,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.8172473596406608</v>
+        <v>0.7993589212817458</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -2992,7 +2992,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8171357135941566</v>
+        <v>0.7992291934582044</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -3003,7 +3003,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>26206.28919791371</v>
+        <v>24762.09664954654</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -3014,7 +3014,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>26274.41519794855</v>
+        <v>24829.02284139164</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -3025,7 +3025,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.2312089853213282</v>
+        <v>0.2025734349744551</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>

</xml_diff>